<commit_message>
Clean up discography files
</commit_message>
<xml_diff>
--- a/src/assets/logickal-discography-FINAL.xlsx
+++ b/src/assets/logickal-discography-FINAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy.dickens/Dev/experimental/logickal-astro/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{887C6C2C-17C7-3D4D-AAAC-95093E9ABB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4C3D1A9D-8004-684D-960D-796055CC09F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{2FA35B67-B640-1246-A9A2-A4C3B33D89DF}"/>
+    <workbookView xWindow="1140" yWindow="4020" windowWidth="28040" windowHeight="17440" xr2:uid="{2FA35B67-B640-1246-A9A2-A4C3B33D89DF}"/>
   </bookViews>
   <sheets>
     <sheet name="logickal-discography" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="255">
   <si>
     <t>title</t>
   </si>
@@ -635,9 +635,6 @@
     <t>https://www.beatport.com/release/rndz/3860307</t>
   </si>
   <si>
-    <t>Orbital Techno Mechanics</t>
-  </si>
-  <si>
     <t>Twelve Offerings</t>
   </si>
   <si>
@@ -792,6 +789,75 @@
   </si>
   <si>
     <t>https://logickal.bandcamp.com/album/phasing-burn-i</t>
+  </si>
+  <si>
+    <t>Techno to dispel obstruction</t>
+  </si>
+  <si>
+    <t>catalogNumber</t>
+  </si>
+  <si>
+    <t>Orbital Mekanik</t>
+  </si>
+  <si>
+    <t>OFFN013</t>
+  </si>
+  <si>
+    <t>OFFN012</t>
+  </si>
+  <si>
+    <t>OFFN011</t>
+  </si>
+  <si>
+    <t>OFFN010</t>
+  </si>
+  <si>
+    <t>OFFN008</t>
+  </si>
+  <si>
+    <t>OFFN009</t>
+  </si>
+  <si>
+    <t>OFFN006</t>
+  </si>
+  <si>
+    <t>OFFN005</t>
+  </si>
+  <si>
+    <t>OFFN004</t>
+  </si>
+  <si>
+    <t>OFFN003</t>
+  </si>
+  <si>
+    <t>OFFN002</t>
+  </si>
+  <si>
+    <t>OFFN001</t>
+  </si>
+  <si>
+    <t>ind</t>
+  </si>
+  <si>
+    <t>drn</t>
+  </si>
+  <si>
+    <t>amb</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>ind,amb</t>
+  </si>
+  <si>
+    <t>ind,drn</t>
+  </si>
+  <si>
+    <t>Music and Production by J. Dickens.  Concept and art by Wright Lagrone</t>
+  </si>
+  <si>
+    <t>Music by J. Dickens</t>
   </si>
 </sst>
 </file>
@@ -1656,20 +1722,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41D618-D66E-6343-90C2-7BD17F86EE78}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="4" width="11" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="35.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1677,496 +1749,562 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>45471</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
       <c r="J2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N2">
         <v>1957328024</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>45401</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>31</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>248</v>
+      </c>
+      <c r="N3">
         <v>636850280</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1">
         <v>45212</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>38</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="M4">
+      <c r="M4" t="s">
+        <v>249</v>
+      </c>
+      <c r="N4">
         <v>3669942547</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="1">
         <v>45212</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>48</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>50</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>51</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="M5">
+      <c r="M5" t="s">
+        <v>247</v>
+      </c>
+      <c r="N5">
         <v>2178494118</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="1">
         <v>45142</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>56</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>47</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>57</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>58</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>59</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>60</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>20</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>21</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="s">
+        <v>249</v>
+      </c>
+      <c r="N6">
         <v>767029377</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>61</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>63</v>
       </c>
       <c r="B7" s="1">
         <v>44988</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>66</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>67</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>68</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>69</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>70</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>20</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="M7">
+      <c r="M7" t="s">
+        <v>251</v>
+      </c>
+      <c r="N7">
         <v>1719331390</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>73</v>
       </c>
       <c r="B8" s="1">
         <v>44897</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>75</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>76</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>77</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>78</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>79</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>80</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>20</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>21</v>
       </c>
-      <c r="M8">
+      <c r="M8" t="s">
+        <v>251</v>
+      </c>
+      <c r="N8">
         <v>3902214331</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>83</v>
       </c>
       <c r="B9" s="1">
         <v>44636</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>85</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>86</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>87</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>88</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>89</v>
       </c>
+      <c r="M9" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
       <c r="B10" s="1">
         <v>44764</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" t="s">
         <v>91</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>92</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>93</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>95</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>96</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>97</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>20</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>21</v>
       </c>
-      <c r="M10">
+      <c r="M10" t="s">
+        <v>247</v>
+      </c>
+      <c r="N10">
         <v>1593268127</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>98</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>100</v>
       </c>
       <c r="B11" s="1">
         <v>44470</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" t="s">
         <v>101</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>102</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>103</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>104</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>105</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>106</v>
       </c>
+      <c r="M11" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="1">
         <v>44323</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" t="s">
         <v>108</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>109</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>110</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>111</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>112</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>113</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>20</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>21</v>
       </c>
-      <c r="M12">
+      <c r="M12" t="s">
+        <v>247</v>
+      </c>
+      <c r="N12">
         <v>4177785744</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="1">
         <v>44270</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" t="s">
         <v>116</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>117</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>118</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -2175,545 +2313,625 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
         <v>119</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>88</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>89</v>
       </c>
-      <c r="M13">
+      <c r="M13" t="s">
+        <v>247</v>
+      </c>
+      <c r="N13">
         <v>1743691083</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>122</v>
       </c>
       <c r="B14" s="1">
         <v>43952</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" t="s">
         <v>123</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>124</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>125</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>126</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>127</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>128</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>20</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>21</v>
       </c>
-      <c r="M14">
+      <c r="M14" t="s">
+        <v>249</v>
+      </c>
+      <c r="N14">
         <v>1482564824</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>131</v>
       </c>
       <c r="B15" s="1">
         <v>43893</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" t="s">
         <v>132</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>133</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>134</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>135</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>136</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>137</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>138</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>88</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>89</v>
       </c>
-      <c r="M15">
+      <c r="M15" t="s">
+        <v>250</v>
+      </c>
+      <c r="N15">
         <v>2921581016</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>139</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>141</v>
       </c>
       <c r="B16" s="1">
         <v>43893</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" t="s">
         <v>142</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>143</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>144</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>145</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>146</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>147</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>148</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>88</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>89</v>
       </c>
-      <c r="M16">
+      <c r="M16" t="s">
+        <v>250</v>
+      </c>
+      <c r="N16">
         <v>3331570853</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>150</v>
       </c>
       <c r="B17" s="1">
         <v>43638</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" t="s">
         <v>151</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>152</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>153</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>154</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>88</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>89</v>
       </c>
+      <c r="M17" t="s">
+        <v>250</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>155</v>
       </c>
       <c r="B18" s="1">
         <v>43555</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" t="s">
         <v>156</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>157</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>158</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>159</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>160</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>161</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>162</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>88</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>89</v>
       </c>
-      <c r="M18">
+      <c r="M18" t="s">
+        <v>247</v>
+      </c>
+      <c r="N18">
         <v>92379576</v>
       </c>
+      <c r="O18" s="2" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>163</v>
       </c>
       <c r="B19" s="1">
         <v>43238</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D19" t="s">
         <v>164</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>165</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>166</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>167</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>168</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>169</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>170</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>20</v>
       </c>
-      <c r="M19">
+      <c r="M19" t="s">
+        <v>248</v>
+      </c>
+      <c r="N19">
         <v>764686814</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>171</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="P19" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>173</v>
       </c>
       <c r="B20" s="1">
         <v>43018</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20" t="s">
         <v>174</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>175</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>176</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>177</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>178</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>179</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
+        <v>234</v>
+      </c>
+      <c r="K20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" t="s">
+        <v>250</v>
+      </c>
+      <c r="N20">
+        <v>2544508314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>180</v>
-      </c>
-      <c r="J20" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20">
-        <v>2544508314</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>181</v>
       </c>
       <c r="B21">
         <v>2007</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" t="s">
         <v>182</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>183</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>184</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>185</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>186</v>
       </c>
-      <c r="J21" t="s">
+      <c r="M21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>188</v>
       </c>
       <c r="B22">
         <v>2006</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+      <c r="G22" t="s">
         <v>189</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>190</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>191</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>192</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
+        <v>186</v>
+      </c>
+      <c r="M22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>193</v>
-      </c>
-      <c r="J22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>194</v>
       </c>
       <c r="B23">
         <v>2006</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G23" t="s">
         <v>195</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>196</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
+        <v>191</v>
+      </c>
+      <c r="J23" t="s">
         <v>197</v>
       </c>
-      <c r="H23" t="s">
-        <v>192</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
+        <v>186</v>
+      </c>
+      <c r="M23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>198</v>
-      </c>
-      <c r="J23" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>199</v>
       </c>
       <c r="B24">
         <v>2008</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>199</v>
+      </c>
+      <c r="G24" t="s">
         <v>200</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>201</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>202</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>203</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
+        <v>186</v>
+      </c>
+      <c r="M24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>204</v>
-      </c>
-      <c r="J24" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>205</v>
       </c>
       <c r="B25">
         <v>2008</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>205</v>
+      </c>
+      <c r="G25" t="s">
         <v>206</v>
       </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
         <v>207</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>208</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>209</v>
       </c>
-      <c r="J25" t="s">
+      <c r="M25" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>211</v>
       </c>
       <c r="B26">
         <v>6692332</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>211</v>
+      </c>
+      <c r="E26" t="s">
         <v>212</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>213</v>
       </c>
-      <c r="E26" t="s">
+      <c r="J26" t="s">
         <v>214</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>215</v>
-      </c>
-      <c r="J26" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>216</v>
       </c>
       <c r="B27" s="1">
         <v>44857</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" t="s">
         <v>217</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>218</v>
       </c>
-      <c r="E27" t="s">
+      <c r="J27" t="s">
         <v>219</v>
       </c>
-      <c r="I27" t="s">
-        <v>220</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>20</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>21</v>
       </c>
+      <c r="M27" t="s">
+        <v>249</v>
+      </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20211023</v>
       </c>
       <c r="B28" s="1">
         <v>44492</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1"/>
+      <c r="D28">
         <v>20211023</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>220</v>
+      </c>
+      <c r="F28" t="s">
         <v>221</v>
       </c>
-      <c r="E28" t="s">
+      <c r="J28" t="s">
         <v>222</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>223</v>
-      </c>
-      <c r="J28" t="s">
-        <v>20</v>
-      </c>
-      <c r="K28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>224</v>
       </c>
       <c r="B29" s="1">
         <v>44196</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" t="s">
+        <v>224</v>
+      </c>
+      <c r="E29" t="s">
         <v>225</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>226</v>
       </c>
-      <c r="E29" t="s">
+      <c r="J29" t="s">
         <v>227</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
+        <v>20</v>
+      </c>
+      <c r="L29" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>228</v>
-      </c>
-      <c r="J29" t="s">
-        <v>20</v>
-      </c>
-      <c r="K29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>229</v>
       </c>
       <c r="B30" s="1">
         <v>44146</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" t="s">
+        <v>229</v>
+      </c>
+      <c r="E30" t="s">
         <v>230</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
         <v>231</v>
       </c>
-      <c r="E30" t="s">
-        <v>232</v>
-      </c>
-      <c r="I30" t="s">
-        <v>228</v>
-      </c>
       <c r="J30" t="s">
+        <v>227</v>
+      </c>
+      <c r="K30" t="s">
         <v>20</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>21</v>
+      </c>
+      <c r="M30" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Building discography pages from xlsx
</commit_message>
<xml_diff>
--- a/src/assets/logickal-discography-FINAL.xlsx
+++ b/src/assets/logickal-discography-FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy.dickens/Dev/experimental/logickal-astro/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4C3D1A9D-8004-684D-960D-796055CC09F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{61809339-66B0-7D47-BCCE-07F937D9D34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="4020" windowWidth="28040" windowHeight="17440" xr2:uid="{2FA35B67-B640-1246-A9A2-A4C3B33D89DF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="255">
   <si>
     <t>title</t>
   </si>
@@ -1724,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41D618-D66E-6343-90C2-7BD17F86EE78}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2306,15 +2306,6 @@
       <c r="F13" t="s">
         <v>118</v>
       </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" t="s">
-        <v>19</v>
-      </c>
       <c r="J13" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
Fix dates and data from XLS
</commit_message>
<xml_diff>
--- a/src/assets/logickal-discography-FINAL.xlsx
+++ b/src/assets/logickal-discography-FINAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy.dickens/Dev/experimental/logickal-astro/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{61809339-66B0-7D47-BCCE-07F937D9D34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{77AA3F8C-9D35-B742-A49B-86533E3E095D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="4020" windowWidth="28040" windowHeight="17440" xr2:uid="{2FA35B67-B640-1246-A9A2-A4C3B33D89DF}"/>
+    <workbookView xWindow="1140" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{2FA35B67-B640-1246-A9A2-A4C3B33D89DF}"/>
   </bookViews>
   <sheets>
     <sheet name="logickal-discography" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="260">
   <si>
     <t>title</t>
   </si>
@@ -454,9 +454,6 @@
     <t>April</t>
   </si>
   <si>
-    <t>ÔøΩaprilÔøΩ</t>
-  </si>
-  <si>
     <t>https://f4.bcbits.com/img/a2611415522_2.jpg</t>
   </si>
   <si>
@@ -710,9 +707,6 @@
     <t>Live at Buzz &amp; Click IV</t>
   </si>
   <si>
-    <t>Live-buzz-click-iv</t>
-  </si>
-  <si>
     <t>https://open.spotify.com/album/0vpL7E8Uh7HFbWg2PXp3hB?si=2qKGUGHiQNiV4JbrK4rSHw</t>
   </si>
   <si>
@@ -858,12 +852,36 @@
   </si>
   <si>
     <t>Music by J. Dickens</t>
+  </si>
+  <si>
+    <t>othersuns</t>
+  </si>
+  <si>
+    <t>OFFS008</t>
+  </si>
+  <si>
+    <t>https://f4.bcbits.com/img/a3838645376_10.jpg</t>
+  </si>
+  <si>
+    <t>Solstice Ritual 2023</t>
+  </si>
+  <si>
+    <t>solstice-ritual-2023</t>
+  </si>
+  <si>
+    <t>april</t>
+  </si>
+  <si>
+    <t>live-buzz-click-iv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1341,12 +1359,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1722,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41D618-D66E-6343-90C2-7BD17F86EE78}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1749,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1795,11 +1815,11 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>45471</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1814,7 +1834,7 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K2" t="s">
         <v>20</v>
@@ -1823,7 +1843,7 @@
         <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N2">
         <v>1957328024</v>
@@ -1839,11 +1859,11 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>45401</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -1873,7 +1893,7 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="N3">
         <v>636850280</v>
@@ -1889,11 +1909,11 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>45212</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
@@ -1923,7 +1943,7 @@
         <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="N4">
         <v>3669942547</v>
@@ -1939,11 +1959,11 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>45212</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
         <v>45</v>
@@ -1973,7 +1993,7 @@
         <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N5">
         <v>2178494118</v>
@@ -1989,11 +2009,11 @@
       <c r="A6" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>45142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D6" t="s">
         <v>55</v>
@@ -2023,7 +2043,7 @@
         <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="N6">
         <v>767029377</v>
@@ -2039,11 +2059,11 @@
       <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>44988</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
@@ -2073,7 +2093,7 @@
         <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N7">
         <v>1719331390</v>
@@ -2089,11 +2109,11 @@
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>44897</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
         <v>74</v>
@@ -2123,7 +2143,7 @@
         <v>21</v>
       </c>
       <c r="M8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N8">
         <v>3902214331</v>
@@ -2139,7 +2159,7 @@
       <c r="A9" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>44636</v>
       </c>
       <c r="C9" s="1"/>
@@ -2162,18 +2182,18 @@
         <v>89</v>
       </c>
       <c r="M9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>44764</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D10" t="s">
         <v>91</v>
@@ -2203,7 +2223,7 @@
         <v>21</v>
       </c>
       <c r="M10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N10">
         <v>1593268127</v>
@@ -2219,7 +2239,7 @@
       <c r="A11" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>44470</v>
       </c>
       <c r="C11" s="1"/>
@@ -2242,18 +2262,18 @@
         <v>106</v>
       </c>
       <c r="M11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>44323</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D12" t="s">
         <v>108</v>
@@ -2280,7 +2300,7 @@
         <v>21</v>
       </c>
       <c r="M12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N12">
         <v>4177785744</v>
@@ -2293,7 +2313,7 @@
       <c r="A13" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>44270</v>
       </c>
       <c r="C13" s="1"/>
@@ -2316,7 +2336,7 @@
         <v>89</v>
       </c>
       <c r="M13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N13">
         <v>1743691083</v>
@@ -2332,29 +2352,29 @@
       <c r="A14" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>43952</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E14" t="s">
         <v>123</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>124</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>125</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>126</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>127</v>
-      </c>
-      <c r="I14" t="s">
-        <v>128</v>
       </c>
       <c r="K14" t="s">
         <v>20</v>
@@ -2363,46 +2383,46 @@
         <v>21</v>
       </c>
       <c r="M14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="N14">
         <v>1482564824</v>
       </c>
       <c r="O14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="P14" t="s">
         <v>129</v>
-      </c>
-      <c r="P14" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B15" s="1">
+        <v>130</v>
+      </c>
+      <c r="B15" s="3">
         <v>43893</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" t="s">
         <v>132</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>133</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>134</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>135</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>136</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>137</v>
-      </c>
-      <c r="J15" t="s">
-        <v>138</v>
       </c>
       <c r="K15" t="s">
         <v>88</v>
@@ -2411,46 +2431,46 @@
         <v>89</v>
       </c>
       <c r="M15" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N15">
         <v>2921581016</v>
       </c>
       <c r="O15" t="s">
+        <v>138</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B16" s="1">
+        <v>140</v>
+      </c>
+      <c r="B16" s="3">
         <v>43893</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" t="s">
         <v>142</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>143</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>144</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>145</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>146</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>147</v>
-      </c>
-      <c r="J16" t="s">
-        <v>148</v>
       </c>
       <c r="K16" t="s">
         <v>88</v>
@@ -2459,34 +2479,34 @@
         <v>89</v>
       </c>
       <c r="M16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N16">
         <v>3331570853</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="1">
+        <v>149</v>
+      </c>
+      <c r="B17" s="3">
         <v>43638</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" t="s">
         <v>151</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>152</v>
       </c>
-      <c r="F17" t="s">
+      <c r="J17" t="s">
         <v>153</v>
-      </c>
-      <c r="J17" t="s">
-        <v>154</v>
       </c>
       <c r="K17" t="s">
         <v>88</v>
@@ -2495,40 +2515,40 @@
         <v>89</v>
       </c>
       <c r="M17" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="1">
+        <v>154</v>
+      </c>
+      <c r="B18" s="3">
         <v>43555</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" t="s">
         <v>156</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>157</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>158</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>159</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>160</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>161</v>
-      </c>
-      <c r="J18" t="s">
-        <v>162</v>
       </c>
       <c r="K18" t="s">
         <v>88</v>
@@ -2537,98 +2557,98 @@
         <v>89</v>
       </c>
       <c r="M18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N18">
         <v>92379576</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="3">
+        <v>43238</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D19" t="s">
         <v>163</v>
       </c>
-      <c r="B19" s="1">
-        <v>43238</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>164</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>165</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>166</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>167</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>168</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>169</v>
-      </c>
-      <c r="J19" t="s">
-        <v>170</v>
       </c>
       <c r="K19" t="s">
         <v>20</v>
       </c>
       <c r="M19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="N19">
         <v>764686814</v>
       </c>
       <c r="O19" t="s">
+        <v>170</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43018</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" t="s">
         <v>173</v>
       </c>
-      <c r="B20" s="1">
-        <v>43018</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>174</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>175</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>176</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>177</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>178</v>
       </c>
-      <c r="I20" t="s">
-        <v>179</v>
-      </c>
       <c r="J20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K20" t="s">
         <v>20</v>
       </c>
       <c r="M20" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N20">
         <v>2544508314</v>
@@ -2636,164 +2656,164 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="3">
+        <v>39401</v>
+      </c>
+      <c r="D21" t="s">
         <v>180</v>
       </c>
-      <c r="B21">
-        <v>2007</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="G21" t="s">
         <v>181</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>182</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>183</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>184</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>185</v>
       </c>
-      <c r="K21" t="s">
-        <v>186</v>
-      </c>
       <c r="M21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="3">
+        <v>39195</v>
+      </c>
+      <c r="D22" t="s">
         <v>187</v>
       </c>
-      <c r="B22">
-        <v>2006</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="G22" t="s">
         <v>188</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>189</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>190</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>191</v>
       </c>
-      <c r="J22" t="s">
-        <v>192</v>
-      </c>
       <c r="K22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="3">
+        <v>38860</v>
+      </c>
+      <c r="D23" t="s">
         <v>193</v>
       </c>
-      <c r="B23">
-        <v>2006</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>194</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>195</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>190</v>
+      </c>
+      <c r="J23" t="s">
         <v>196</v>
       </c>
-      <c r="I23" t="s">
-        <v>191</v>
-      </c>
-      <c r="J23" t="s">
-        <v>197</v>
-      </c>
       <c r="K23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" s="3">
+        <v>39665</v>
+      </c>
+      <c r="D24" t="s">
         <v>198</v>
       </c>
-      <c r="B24">
-        <v>2008</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>199</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>200</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>201</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>202</v>
       </c>
-      <c r="J24" t="s">
-        <v>203</v>
-      </c>
       <c r="K24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="3">
+        <v>39567</v>
+      </c>
+      <c r="D25" t="s">
+        <v>259</v>
+      </c>
+      <c r="G25" t="s">
         <v>204</v>
       </c>
-      <c r="B25">
-        <v>2008</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="H25" t="s">
         <v>205</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>206</v>
       </c>
-      <c r="H25" t="s">
+      <c r="K25" t="s">
         <v>207</v>
       </c>
-      <c r="J25" t="s">
-        <v>208</v>
-      </c>
-      <c r="K25" t="s">
-        <v>209</v>
-      </c>
       <c r="M25" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="3">
+        <v>44919</v>
+      </c>
+      <c r="D26" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" t="s">
         <v>210</v>
       </c>
-      <c r="B26">
-        <v>6692332</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>211</v>
       </c>
-      <c r="E26" t="s">
+      <c r="J26" t="s">
         <v>212</v>
-      </c>
-      <c r="F26" t="s">
-        <v>213</v>
-      </c>
-      <c r="J26" t="s">
-        <v>214</v>
       </c>
       <c r="K26" t="s">
         <v>20</v>
@@ -2802,28 +2822,28 @@
         <v>21</v>
       </c>
       <c r="M26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>215</v>
-      </c>
-      <c r="B27" s="1">
+        <v>213</v>
+      </c>
+      <c r="B27" s="3">
         <v>44857</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
+        <v>214</v>
+      </c>
+      <c r="E27" t="s">
+        <v>215</v>
+      </c>
+      <c r="F27" t="s">
         <v>216</v>
       </c>
-      <c r="E27" t="s">
+      <c r="J27" t="s">
         <v>217</v>
-      </c>
-      <c r="F27" t="s">
-        <v>218</v>
-      </c>
-      <c r="J27" t="s">
-        <v>219</v>
       </c>
       <c r="K27" t="s">
         <v>20</v>
@@ -2832,14 +2852,14 @@
         <v>21</v>
       </c>
       <c r="M27" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="4">
         <v>20211023</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="3">
         <v>44492</v>
       </c>
       <c r="C28" s="1"/>
@@ -2847,13 +2867,13 @@
         <v>20211023</v>
       </c>
       <c r="E28" t="s">
+        <v>218</v>
+      </c>
+      <c r="F28" t="s">
+        <v>219</v>
+      </c>
+      <c r="J28" t="s">
         <v>220</v>
-      </c>
-      <c r="F28" t="s">
-        <v>221</v>
-      </c>
-      <c r="J28" t="s">
-        <v>222</v>
       </c>
       <c r="K28" t="s">
         <v>20</v>
@@ -2862,28 +2882,28 @@
         <v>21</v>
       </c>
       <c r="M28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>223</v>
-      </c>
-      <c r="B29" s="1">
+        <v>221</v>
+      </c>
+      <c r="B29" s="3">
         <v>44196</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E29" t="s">
+        <v>223</v>
+      </c>
+      <c r="F29" t="s">
         <v>224</v>
       </c>
-      <c r="E29" t="s">
+      <c r="J29" t="s">
         <v>225</v>
-      </c>
-      <c r="F29" t="s">
-        <v>226</v>
-      </c>
-      <c r="J29" t="s">
-        <v>227</v>
       </c>
       <c r="K29" t="s">
         <v>20</v>
@@ -2892,28 +2912,28 @@
         <v>21</v>
       </c>
       <c r="M29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>228</v>
-      </c>
-      <c r="B30" s="1">
+        <v>226</v>
+      </c>
+      <c r="B30" s="3">
         <v>44146</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E30" t="s">
+        <v>228</v>
+      </c>
+      <c r="F30" t="s">
         <v>229</v>
       </c>
-      <c r="E30" t="s">
-        <v>230</v>
-      </c>
-      <c r="F30" t="s">
-        <v>231</v>
-      </c>
       <c r="J30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K30" t="s">
         <v>20</v>
@@ -2922,7 +2942,41 @@
         <v>21</v>
       </c>
       <c r="M30" t="s">
-        <v>250</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45153</v>
+      </c>
+      <c r="C31" t="s">
+        <v>254</v>
+      </c>
+      <c r="D31" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" t="s">
+        <v>255</v>
+      </c>
+      <c r="M31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>256</v>
+      </c>
+      <c r="B32" s="3">
+        <v>45281</v>
+      </c>
+      <c r="D32" t="s">
+        <v>257</v>
+      </c>
+      <c r="M32" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial work on discography categories
</commit_message>
<xml_diff>
--- a/src/assets/logickal-discography-FINAL.xlsx
+++ b/src/assets/logickal-discography-FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy.dickens/Dev/experimental/logickal-astro/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{77AA3F8C-9D35-B742-A49B-86533E3E095D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{91BFD67C-4A0A-194F-BB0C-5820900092F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{2FA35B67-B640-1246-A9A2-A4C3B33D89DF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="263">
   <si>
     <t>title</t>
   </si>
@@ -530,9 +530,6 @@
     <t>https://www.beatport.com/release/senkan/3860321</t>
   </si>
   <si>
-    <t>ÔøΩSenkanÔøΩ C/W ÔøΩBraking Gate (rmx)ÔøΩ</t>
-  </si>
-  <si>
     <t>All instruments/production barely controlled by J. Dickens_x000D_
 _x000D_
 All proceeds from this record will be donated to The Community Foundation of Middle Tennessee to support disaster recovery in the wake of the tornadoes that impacted our community on March 3, 2020. _x000D_
@@ -873,6 +870,18 @@
   </si>
   <si>
     <t>live-buzz-click-iv</t>
+  </si>
+  <si>
+    <t>A companion piece of tracks associated with SOLIS.</t>
+  </si>
+  <si>
+    <t>A solstice gift for Bandcamp Subscribers in 2023.</t>
+  </si>
+  <si>
+    <t>FM Drones for Springtime</t>
+  </si>
+  <si>
+    <t>Part of the 2020 March Is For Singles series</t>
   </si>
 </sst>
 </file>
@@ -1744,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41D618-D66E-6343-90C2-7BD17F86EE78}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1769,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1819,7 +1828,7 @@
         <v>45471</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1834,7 +1843,7 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K2" t="s">
         <v>20</v>
@@ -1843,7 +1852,7 @@
         <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N2">
         <v>1957328024</v>
@@ -1863,7 +1872,7 @@
         <v>45401</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -1893,7 +1902,7 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N3">
         <v>636850280</v>
@@ -1913,7 +1922,7 @@
         <v>45212</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
@@ -1943,7 +1952,7 @@
         <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N4">
         <v>3669942547</v>
@@ -1963,7 +1972,7 @@
         <v>45212</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" t="s">
         <v>45</v>
@@ -1993,7 +2002,7 @@
         <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N5">
         <v>2178494118</v>
@@ -2013,7 +2022,7 @@
         <v>45142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
         <v>55</v>
@@ -2043,7 +2052,7 @@
         <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N6">
         <v>767029377</v>
@@ -2063,7 +2072,7 @@
         <v>44988</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
@@ -2093,7 +2102,7 @@
         <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N7">
         <v>1719331390</v>
@@ -2113,7 +2122,7 @@
         <v>44897</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" t="s">
         <v>74</v>
@@ -2143,7 +2152,7 @@
         <v>21</v>
       </c>
       <c r="M8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N8">
         <v>3902214331</v>
@@ -2182,7 +2191,7 @@
         <v>89</v>
       </c>
       <c r="M9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -2193,7 +2202,7 @@
         <v>44764</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D10" t="s">
         <v>91</v>
@@ -2223,7 +2232,7 @@
         <v>21</v>
       </c>
       <c r="M10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N10">
         <v>1593268127</v>
@@ -2262,7 +2271,7 @@
         <v>106</v>
       </c>
       <c r="M11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -2273,7 +2282,7 @@
         <v>44323</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D12" t="s">
         <v>108</v>
@@ -2300,7 +2309,7 @@
         <v>21</v>
       </c>
       <c r="M12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N12">
         <v>4177785744</v>
@@ -2336,7 +2345,7 @@
         <v>89</v>
       </c>
       <c r="M13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N13">
         <v>1743691083</v>
@@ -2356,10 +2365,10 @@
         <v>43952</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E14" t="s">
         <v>123</v>
@@ -2376,6 +2385,9 @@
       <c r="I14" t="s">
         <v>127</v>
       </c>
+      <c r="J14" t="s">
+        <v>261</v>
+      </c>
       <c r="K14" t="s">
         <v>20</v>
       </c>
@@ -2383,7 +2395,7 @@
         <v>21</v>
       </c>
       <c r="M14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N14">
         <v>1482564824</v>
@@ -2431,7 +2443,7 @@
         <v>89</v>
       </c>
       <c r="M15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N15">
         <v>2921581016</v>
@@ -2470,7 +2482,7 @@
         <v>146</v>
       </c>
       <c r="J16" t="s">
-        <v>147</v>
+        <v>262</v>
       </c>
       <c r="K16" t="s">
         <v>88</v>
@@ -2479,34 +2491,34 @@
         <v>89</v>
       </c>
       <c r="M16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N16">
         <v>3331570853</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="3">
         <v>43638</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" t="s">
         <v>150</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>151</v>
       </c>
-      <c r="F17" t="s">
+      <c r="J17" t="s">
         <v>152</v>
-      </c>
-      <c r="J17" t="s">
-        <v>153</v>
       </c>
       <c r="K17" t="s">
         <v>88</v>
@@ -2515,40 +2527,40 @@
         <v>89</v>
       </c>
       <c r="M17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B18" s="3">
         <v>43555</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" t="s">
         <v>155</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>156</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>157</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>158</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>159</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>160</v>
-      </c>
-      <c r="J18" t="s">
-        <v>161</v>
       </c>
       <c r="K18" t="s">
         <v>88</v>
@@ -2557,98 +2569,98 @@
         <v>89</v>
       </c>
       <c r="M18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N18">
         <v>92379576</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="3">
         <v>43238</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" t="s">
         <v>163</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>164</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>165</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>166</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>167</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>168</v>
-      </c>
-      <c r="J19" t="s">
-        <v>169</v>
       </c>
       <c r="K19" t="s">
         <v>20</v>
       </c>
       <c r="M19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N19">
         <v>764686814</v>
       </c>
       <c r="O19" t="s">
+        <v>169</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B20" s="3">
         <v>43018</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" t="s">
         <v>173</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>174</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>175</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>176</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>177</v>
       </c>
-      <c r="I20" t="s">
-        <v>178</v>
-      </c>
       <c r="J20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K20" t="s">
         <v>20</v>
       </c>
       <c r="M20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N20">
         <v>2544508314</v>
@@ -2656,164 +2668,164 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B21" s="3">
         <v>39401</v>
       </c>
       <c r="D21" t="s">
+        <v>179</v>
+      </c>
+      <c r="G21" t="s">
         <v>180</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>181</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>182</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>183</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>184</v>
       </c>
-      <c r="K21" t="s">
-        <v>185</v>
-      </c>
       <c r="M21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" s="3">
         <v>39195</v>
       </c>
       <c r="D22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" t="s">
         <v>187</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>188</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>189</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>190</v>
       </c>
-      <c r="J22" t="s">
-        <v>191</v>
-      </c>
       <c r="K22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B23" s="3">
         <v>38860</v>
       </c>
       <c r="D23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G23" t="s">
         <v>193</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>194</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>189</v>
+      </c>
+      <c r="J23" t="s">
         <v>195</v>
       </c>
-      <c r="I23" t="s">
-        <v>190</v>
-      </c>
-      <c r="J23" t="s">
-        <v>196</v>
-      </c>
       <c r="K23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" s="3">
         <v>39665</v>
       </c>
       <c r="D24" t="s">
+        <v>197</v>
+      </c>
+      <c r="G24" t="s">
         <v>198</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>199</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>200</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>201</v>
       </c>
-      <c r="J24" t="s">
-        <v>202</v>
-      </c>
       <c r="K24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="3">
         <v>39567</v>
       </c>
       <c r="D25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G25" t="s">
+        <v>203</v>
+      </c>
+      <c r="H25" t="s">
         <v>204</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J25" t="s">
         <v>205</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>206</v>
       </c>
-      <c r="K25" t="s">
-        <v>207</v>
-      </c>
       <c r="M25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B26" s="3">
         <v>44919</v>
       </c>
       <c r="D26" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" t="s">
         <v>209</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>210</v>
       </c>
-      <c r="F26" t="s">
+      <c r="J26" t="s">
         <v>211</v>
-      </c>
-      <c r="J26" t="s">
-        <v>212</v>
       </c>
       <c r="K26" t="s">
         <v>20</v>
@@ -2822,28 +2834,28 @@
         <v>21</v>
       </c>
       <c r="M26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B27" s="3">
         <v>44857</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
+        <v>213</v>
+      </c>
+      <c r="E27" t="s">
         <v>214</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>215</v>
       </c>
-      <c r="F27" t="s">
+      <c r="J27" t="s">
         <v>216</v>
-      </c>
-      <c r="J27" t="s">
-        <v>217</v>
       </c>
       <c r="K27" t="s">
         <v>20</v>
@@ -2852,7 +2864,7 @@
         <v>21</v>
       </c>
       <c r="M27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
@@ -2867,13 +2879,13 @@
         <v>20211023</v>
       </c>
       <c r="E28" t="s">
+        <v>217</v>
+      </c>
+      <c r="F28" t="s">
         <v>218</v>
       </c>
-      <c r="F28" t="s">
+      <c r="J28" t="s">
         <v>219</v>
-      </c>
-      <c r="J28" t="s">
-        <v>220</v>
       </c>
       <c r="K28" t="s">
         <v>20</v>
@@ -2882,28 +2894,28 @@
         <v>21</v>
       </c>
       <c r="M28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B29" s="3">
         <v>44196</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" t="s">
         <v>222</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>223</v>
       </c>
-      <c r="F29" t="s">
+      <c r="J29" t="s">
         <v>224</v>
-      </c>
-      <c r="J29" t="s">
-        <v>225</v>
       </c>
       <c r="K29" t="s">
         <v>20</v>
@@ -2912,28 +2924,28 @@
         <v>21</v>
       </c>
       <c r="M29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B30" s="3">
         <v>44146</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" t="s">
+        <v>226</v>
+      </c>
+      <c r="E30" t="s">
         <v>227</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>228</v>
       </c>
-      <c r="F30" t="s">
-        <v>229</v>
-      </c>
       <c r="J30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K30" t="s">
         <v>20</v>
@@ -2942,41 +2954,59 @@
         <v>21</v>
       </c>
       <c r="M30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B31" s="3">
         <v>45153</v>
       </c>
       <c r="C31" t="s">
+        <v>253</v>
+      </c>
+      <c r="D31" t="s">
+        <v>252</v>
+      </c>
+      <c r="E31" t="s">
         <v>254</v>
       </c>
-      <c r="D31" t="s">
-        <v>253</v>
-      </c>
-      <c r="E31" t="s">
-        <v>255</v>
+      <c r="J31" t="s">
+        <v>259</v>
+      </c>
+      <c r="K31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" t="s">
+        <v>21</v>
       </c>
       <c r="M31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B32" s="3">
         <v>45281</v>
       </c>
       <c r="D32" t="s">
-        <v>257</v>
+        <v>256</v>
+      </c>
+      <c r="J32" t="s">
+        <v>260</v>
+      </c>
+      <c r="K32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" t="s">
+        <v>21</v>
       </c>
       <c r="M32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add updates to discography and discogCard component
</commit_message>
<xml_diff>
--- a/src/assets/logickal-discography-FINAL.xlsx
+++ b/src/assets/logickal-discography-FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy.dickens/Dev/experimental/logickal-astro/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F10024-F9A6-2941-ABDD-A1EC6F4E4360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A88369-68B9-9B4A-BE98-9C600A7FCFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{2FA35B67-B640-1246-A9A2-A4C3B33D89DF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="267">
   <si>
     <t>title</t>
   </si>
@@ -882,6 +882,18 @@
   </si>
   <si>
     <t>senkan</t>
+  </si>
+  <si>
+    <t>Tranquillitatis</t>
+  </si>
+  <si>
+    <t>OFFN014</t>
+  </si>
+  <si>
+    <t>tranquillitatis</t>
+  </si>
+  <si>
+    <t>Music for moonwalkers I</t>
   </si>
 </sst>
 </file>
@@ -1751,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A41D618-D66E-6343-90C2-7BD17F86EE78}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1820,30 +1832,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3">
-        <v>45471</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>231</v>
+        <v>263</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45506</v>
+      </c>
+      <c r="C2" t="s">
+        <v>264</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
+        <v>265</v>
       </c>
       <c r="J2" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
       <c r="K2" t="s">
         <v>20</v>
@@ -1852,48 +1855,33 @@
         <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>247</v>
-      </c>
-      <c r="N2">
-        <v>1957328024</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
-        <v>45401</v>
+        <v>45471</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>228</v>
       </c>
       <c r="K3" t="s">
         <v>20</v>
@@ -1902,48 +1890,48 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="N3">
-        <v>636850280</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
+        <v>1957328024</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3">
-        <v>45212</v>
+        <v>45401</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
         <v>20</v>
@@ -1952,48 +1940,48 @@
         <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N4">
-        <v>3669942547</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" t="s">
-        <v>43</v>
+        <v>636850280</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <v>45212</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="K5" t="s">
         <v>20</v>
@@ -2002,48 +1990,48 @@
         <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="N5">
-        <v>2178494118</v>
+        <v>3669942547</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
-        <v>45142</v>
+        <v>45212</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
         <v>20</v>
@@ -2052,48 +2040,48 @@
         <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N6">
-        <v>767029377</v>
-      </c>
-      <c r="O6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P6" t="s">
-        <v>62</v>
+        <v>2178494118</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3">
-        <v>44988</v>
+        <v>45142</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="K7" t="s">
         <v>20</v>
@@ -2102,48 +2090,48 @@
         <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="N7">
-        <v>1719331390</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>72</v>
+        <v>767029377</v>
+      </c>
+      <c r="O7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3">
-        <v>44897</v>
+        <v>44988</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="K8" t="s">
         <v>20</v>
@@ -2155,334 +2143,336 @@
         <v>261</v>
       </c>
       <c r="N8">
-        <v>3902214331</v>
+        <v>1719331390</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3">
-        <v>44636</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>44897</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>237</v>
+      </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>76</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" t="s">
+        <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K9" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="M9" t="s">
-        <v>243</v>
+        <v>261</v>
+      </c>
+      <c r="N9">
+        <v>3902214331</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3">
-        <v>44764</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>238</v>
-      </c>
+        <v>44636</v>
+      </c>
+      <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="J10" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="M10" t="s">
         <v>243</v>
       </c>
-      <c r="N10">
-        <v>1593268127</v>
-      </c>
-      <c r="O10" t="s">
-        <v>98</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B11" s="3">
-        <v>44470</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>44764</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>93</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
+        <v>96</v>
       </c>
       <c r="J11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="K11" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="M11" t="s">
         <v>243</v>
       </c>
+      <c r="N11">
+        <v>1593268127</v>
+      </c>
+      <c r="O11" t="s">
+        <v>98</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B12" s="3">
-        <v>44323</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>239</v>
-      </c>
+        <v>44470</v>
+      </c>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F12" t="s">
-        <v>110</v>
-      </c>
-      <c r="G12" t="s">
-        <v>111</v>
-      </c>
-      <c r="H12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12" t="s">
-        <v>113</v>
+        <v>103</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
       </c>
       <c r="K12" t="s">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="M12" t="s">
         <v>243</v>
       </c>
-      <c r="N12">
-        <v>4177785744</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B13" s="3">
-        <v>44270</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>44323</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
-      </c>
-      <c r="J13" t="s">
-        <v>119</v>
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" t="s">
+        <v>113</v>
       </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="M13" t="s">
         <v>243</v>
       </c>
       <c r="N13">
-        <v>1743691083</v>
+        <v>4177785744</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="P13" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B14" s="3">
-        <v>43952</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>240</v>
-      </c>
+        <v>44270</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" t="s">
-        <v>255</v>
+        <v>116</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H14" t="s">
-        <v>126</v>
-      </c>
-      <c r="I14" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="J14" t="s">
-        <v>259</v>
+        <v>119</v>
       </c>
       <c r="K14" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="M14" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N14">
-        <v>1482564824</v>
+        <v>1743691083</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="P14" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B15" s="3">
-        <v>43893</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>43952</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>240</v>
+      </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>255</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G15" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I15" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="J15" t="s">
-        <v>137</v>
+        <v>259</v>
       </c>
       <c r="K15" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="M15" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N15">
-        <v>2921581016</v>
-      </c>
-      <c r="O15" t="s">
-        <v>138</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>139</v>
+        <v>1482564824</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="P15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B16" s="3">
         <v>43893</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F16" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="I16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="J16" t="s">
-        <v>260</v>
+        <v>137</v>
       </c>
       <c r="K16" t="s">
         <v>88</v>
@@ -2494,31 +2484,43 @@
         <v>245</v>
       </c>
       <c r="N16">
-        <v>3331570853</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+        <v>2921581016</v>
+      </c>
+      <c r="O16" t="s">
+        <v>138</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B17" s="3">
-        <v>43638</v>
+        <v>43893</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>262</v>
       </c>
       <c r="E17" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F17" t="s">
-        <v>150</v>
+        <v>142</v>
+      </c>
+      <c r="G17" t="s">
+        <v>143</v>
+      </c>
+      <c r="H17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" t="s">
+        <v>145</v>
       </c>
       <c r="J17" t="s">
-        <v>151</v>
+        <v>260</v>
       </c>
       <c r="K17" t="s">
         <v>88</v>
@@ -2527,40 +2529,34 @@
         <v>89</v>
       </c>
       <c r="M17" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="N17">
+        <v>3331570853</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B18" s="3">
-        <v>43555</v>
+        <v>43638</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F18" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" t="s">
-        <v>156</v>
-      </c>
-      <c r="H18" t="s">
-        <v>157</v>
-      </c>
-      <c r="I18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="J18" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="K18" t="s">
         <v>88</v>
@@ -2569,182 +2565,195 @@
         <v>89</v>
       </c>
       <c r="M18" t="s">
+        <v>246</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="3">
+        <v>43555</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" t="s">
+        <v>88</v>
+      </c>
+      <c r="L19" t="s">
+        <v>89</v>
+      </c>
+      <c r="M19" t="s">
         <v>243</v>
       </c>
-      <c r="N18">
+      <c r="N19">
         <v>92379576</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>160</v>
-      </c>
-      <c r="B19" s="3">
-        <v>43238</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D19" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" t="s">
-        <v>162</v>
-      </c>
-      <c r="F19" t="s">
-        <v>163</v>
-      </c>
-      <c r="G19" t="s">
-        <v>164</v>
-      </c>
-      <c r="H19" t="s">
-        <v>165</v>
-      </c>
-      <c r="I19" t="s">
-        <v>166</v>
-      </c>
-      <c r="J19" t="s">
-        <v>167</v>
-      </c>
-      <c r="K19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" t="s">
-        <v>244</v>
-      </c>
-      <c r="N19">
-        <v>764686814</v>
-      </c>
-      <c r="O19" t="s">
-        <v>168</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B20" s="3">
-        <v>43018</v>
+        <v>43238</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="E20" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F20" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H20" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="I20" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="J20" t="s">
-        <v>230</v>
+        <v>167</v>
       </c>
       <c r="K20" t="s">
         <v>20</v>
       </c>
       <c r="M20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N20">
-        <v>2544508314</v>
+        <v>764686814</v>
+      </c>
+      <c r="O20" t="s">
+        <v>168</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B21" s="3">
-        <v>39401</v>
+        <v>43018</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>171</v>
+      </c>
+      <c r="E21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" t="s">
+        <v>173</v>
       </c>
       <c r="G21" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H21" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I21" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="J21" t="s">
-        <v>182</v>
+        <v>230</v>
       </c>
       <c r="K21" t="s">
-        <v>183</v>
+        <v>20</v>
       </c>
       <c r="M21" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="N21">
+        <v>2544508314</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B22" s="3">
-        <v>39195</v>
+        <v>39401</v>
       </c>
       <c r="D22" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G22" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="H22" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="I22" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="J22" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="K22" t="s">
         <v>183</v>
       </c>
       <c r="M22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B23" s="3">
-        <v>38860</v>
+        <v>39195</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G23" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H23" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="I23" t="s">
         <v>188</v>
       </c>
       <c r="J23" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="K23" t="s">
         <v>183</v>
@@ -2755,25 +2764,25 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B24" s="3">
-        <v>39665</v>
+        <v>38860</v>
       </c>
       <c r="D24" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G24" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H24" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I24" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="J24" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K24" t="s">
         <v>183</v>
@@ -2784,25 +2793,28 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B25" s="3">
-        <v>39567</v>
+        <v>39665</v>
       </c>
       <c r="D25" t="s">
-        <v>256</v>
+        <v>196</v>
       </c>
       <c r="G25" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H25" t="s">
-        <v>203</v>
+        <v>198</v>
+      </c>
+      <c r="I25" t="s">
+        <v>199</v>
       </c>
       <c r="J25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K25" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="M25" t="s">
         <v>246</v>
@@ -2810,52 +2822,48 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B26" s="3">
-        <v>44919</v>
+        <v>39567</v>
       </c>
       <c r="D26" t="s">
-        <v>207</v>
-      </c>
-      <c r="E26" t="s">
-        <v>208</v>
-      </c>
-      <c r="F26" t="s">
-        <v>209</v>
+        <v>256</v>
+      </c>
+      <c r="G26" t="s">
+        <v>202</v>
+      </c>
+      <c r="H26" t="s">
+        <v>203</v>
       </c>
       <c r="J26" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="K26" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="M26" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B27" s="3">
-        <v>44857</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>44919</v>
+      </c>
       <c r="D27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E27" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F27" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="J27" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="K27" t="s">
         <v>20</v>
@@ -2864,28 +2872,28 @@
         <v>21</v>
       </c>
       <c r="M27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>20211023</v>
+      <c r="A28" t="s">
+        <v>211</v>
       </c>
       <c r="B28" s="3">
-        <v>44492</v>
+        <v>44857</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28">
-        <v>20211023</v>
+      <c r="D28" t="s">
+        <v>212</v>
       </c>
       <c r="E28" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F28" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K28" t="s">
         <v>20</v>
@@ -2898,24 +2906,24 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>219</v>
+      <c r="A29" s="4">
+        <v>20211023</v>
       </c>
       <c r="B29" s="3">
-        <v>44196</v>
+        <v>44492</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" t="s">
-        <v>220</v>
+      <c r="D29">
+        <v>20211023</v>
       </c>
       <c r="E29" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F29" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J29" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K29" t="s">
         <v>20</v>
@@ -2924,25 +2932,25 @@
         <v>21</v>
       </c>
       <c r="M29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B30" s="3">
-        <v>44146</v>
+        <v>44196</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E30" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F30" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J30" t="s">
         <v>223</v>
@@ -2959,22 +2967,23 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="B31" s="3">
-        <v>45153</v>
-      </c>
-      <c r="C31" t="s">
-        <v>251</v>
-      </c>
+        <v>44146</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="E31" t="s">
-        <v>252</v>
+        <v>226</v>
+      </c>
+      <c r="F31" t="s">
+        <v>227</v>
       </c>
       <c r="J31" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="K31" t="s">
         <v>20</v>
@@ -2983,21 +2992,27 @@
         <v>21</v>
       </c>
       <c r="M31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B32" s="3">
-        <v>45281</v>
+        <v>45153</v>
+      </c>
+      <c r="C32" t="s">
+        <v>251</v>
       </c>
       <c r="D32" t="s">
-        <v>254</v>
+        <v>250</v>
+      </c>
+      <c r="E32" t="s">
+        <v>252</v>
       </c>
       <c r="J32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K32" t="s">
         <v>20</v>
@@ -3006,6 +3021,29 @@
         <v>21</v>
       </c>
       <c r="M32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" s="3">
+        <v>45281</v>
+      </c>
+      <c r="D33" t="s">
+        <v>254</v>
+      </c>
+      <c r="J33" t="s">
+        <v>258</v>
+      </c>
+      <c r="K33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" t="s">
         <v>244</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to discography data
</commit_message>
<xml_diff>
--- a/src/assets/logickal-discography-FINAL.xlsx
+++ b/src/assets/logickal-discography-FINAL.xlsx
@@ -1034,6 +1034,9 @@
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
@@ -1041,9 +1044,6 @@
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2104,7 +2104,8 @@
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="24.3516" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5781" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
     <col min="6" max="6" width="52.1719" style="1" customWidth="1"/>
@@ -2201,11 +2202,13 @@
       <c r="M2" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" t="s" s="5">
+      <c r="N2" s="5">
+        <v>301936655</v>
+      </c>
+      <c r="O2" t="s" s="6">
         <v>24</v>
       </c>
-      <c r="P2" t="s" s="6">
+      <c r="P2" t="s" s="7">
         <v>25</v>
       </c>
     </row>
@@ -2241,11 +2244,13 @@
       <c r="M3" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" t="s" s="5">
+      <c r="N3" s="5">
+        <v>3789870696</v>
+      </c>
+      <c r="O3" t="s" s="6">
         <v>32</v>
       </c>
-      <c r="P3" t="s" s="5">
+      <c r="P3" t="s" s="6">
         <v>33</v>
       </c>
     </row>
@@ -2253,7 +2258,7 @@
       <c r="A4" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <v>45471</v>
       </c>
       <c r="C4" t="s" s="2">
@@ -2287,13 +2292,13 @@
       <c r="M4" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="5">
         <v>1957328024</v>
       </c>
-      <c r="O4" t="s" s="5">
+      <c r="O4" t="s" s="6">
         <v>43</v>
       </c>
-      <c r="P4" t="s" s="5">
+      <c r="P4" t="s" s="6">
         <v>44</v>
       </c>
     </row>
@@ -2301,7 +2306,7 @@
       <c r="A5" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <v>45401</v>
       </c>
       <c r="C5" t="s" s="2">
@@ -2337,13 +2342,13 @@
       <c r="M5" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="5">
         <v>636850280</v>
       </c>
       <c r="O5" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="P5" t="s" s="5">
+      <c r="P5" t="s" s="6">
         <v>56</v>
       </c>
     </row>
@@ -2351,7 +2356,7 @@
       <c r="A6" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <v>45212</v>
       </c>
       <c r="C6" t="s" s="2">
@@ -2387,10 +2392,10 @@
       <c r="M6" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="5">
         <v>3669942547</v>
       </c>
-      <c r="O6" t="s" s="5">
+      <c r="O6" t="s" s="6">
         <v>67</v>
       </c>
       <c r="P6" t="s" s="2">
@@ -2401,7 +2406,7 @@
       <c r="A7" t="s" s="2">
         <v>69</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>45212</v>
       </c>
       <c r="C7" t="s" s="2">
@@ -2437,13 +2442,13 @@
       <c r="M7" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="5">
         <v>2178494118</v>
       </c>
-      <c r="O7" t="s" s="5">
+      <c r="O7" t="s" s="6">
         <v>78</v>
       </c>
-      <c r="P7" t="s" s="5">
+      <c r="P7" t="s" s="6">
         <v>79</v>
       </c>
     </row>
@@ -2451,7 +2456,7 @@
       <c r="A8" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="8">
         <v>45142</v>
       </c>
       <c r="C8" t="s" s="2">
@@ -2487,7 +2492,7 @@
       <c r="M8" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="5">
         <v>767029377</v>
       </c>
       <c r="O8" t="s" s="2">
@@ -2501,7 +2506,7 @@
       <c r="A9" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="8">
         <v>44988</v>
       </c>
       <c r="C9" t="s" s="2">
@@ -2537,13 +2542,13 @@
       <c r="M9" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="5">
         <v>1719331390</v>
       </c>
-      <c r="O9" t="s" s="5">
+      <c r="O9" t="s" s="6">
         <v>100</v>
       </c>
-      <c r="P9" t="s" s="5">
+      <c r="P9" t="s" s="6">
         <v>101</v>
       </c>
     </row>
@@ -2551,7 +2556,7 @@
       <c r="A10" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="8">
         <v>44897</v>
       </c>
       <c r="C10" t="s" s="2">
@@ -2587,13 +2592,13 @@
       <c r="M10" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="5">
         <v>3902214331</v>
       </c>
-      <c r="O10" t="s" s="5">
+      <c r="O10" t="s" s="6">
         <v>111</v>
       </c>
-      <c r="P10" t="s" s="5">
+      <c r="P10" t="s" s="6">
         <v>112</v>
       </c>
     </row>
@@ -2601,7 +2606,7 @@
       <c r="A11" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="8">
         <v>44636</v>
       </c>
       <c r="C11" s="3"/>
@@ -2637,7 +2642,7 @@
       <c r="A12" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="8">
         <v>44764</v>
       </c>
       <c r="C12" t="s" s="2">
@@ -2673,13 +2678,13 @@
       <c r="M12" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="5">
         <v>1593268127</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="P12" t="s" s="5">
+      <c r="P12" t="s" s="6">
         <v>130</v>
       </c>
     </row>
@@ -2687,7 +2692,7 @@
       <c r="A13" t="s" s="2">
         <v>131</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="8">
         <v>44470</v>
       </c>
       <c r="C13" s="3"/>
@@ -2723,7 +2728,7 @@
       <c r="A14" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="8">
         <v>44323</v>
       </c>
       <c r="C14" t="s" s="2">
@@ -2757,10 +2762,10 @@
       <c r="M14" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="5">
         <v>4177785744</v>
       </c>
-      <c r="O14" t="s" s="5">
+      <c r="O14" t="s" s="6">
         <v>146</v>
       </c>
       <c r="P14" s="4"/>
@@ -2769,7 +2774,7 @@
       <c r="A15" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="8">
         <v>44270</v>
       </c>
       <c r="C15" s="3"/>
@@ -2797,10 +2802,10 @@
       <c r="M15" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="5">
         <v>1743691083</v>
       </c>
-      <c r="O15" t="s" s="5">
+      <c r="O15" t="s" s="6">
         <v>152</v>
       </c>
       <c r="P15" t="s" s="2">
@@ -2811,7 +2816,7 @@
       <c r="A16" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="8">
         <v>43952</v>
       </c>
       <c r="C16" t="s" s="2">
@@ -2847,10 +2852,10 @@
       <c r="M16" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="5">
         <v>1482564824</v>
       </c>
-      <c r="O16" t="s" s="5">
+      <c r="O16" t="s" s="6">
         <v>163</v>
       </c>
       <c r="P16" t="s" s="2">
@@ -2861,7 +2866,7 @@
       <c r="A17" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="8">
         <v>43893</v>
       </c>
       <c r="C17" s="3"/>
@@ -2895,13 +2900,13 @@
       <c r="M17" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="5">
         <v>2921581016</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="P17" t="s" s="5">
+      <c r="P17" t="s" s="6">
         <v>174</v>
       </c>
     </row>
@@ -2909,7 +2914,7 @@
       <c r="A18" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="8">
         <v>43893</v>
       </c>
       <c r="C18" s="3"/>
@@ -2943,10 +2948,10 @@
       <c r="M18" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="5">
         <v>3331570853</v>
       </c>
-      <c r="O18" t="s" s="5">
+      <c r="O18" t="s" s="6">
         <v>183</v>
       </c>
       <c r="P18" s="4"/>
@@ -2955,7 +2960,7 @@
       <c r="A19" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="8">
         <v>43638</v>
       </c>
       <c r="C19" s="3"/>
@@ -2984,7 +2989,7 @@
         <v>66</v>
       </c>
       <c r="N19" s="4"/>
-      <c r="O19" t="s" s="5">
+      <c r="O19" t="s" s="6">
         <v>189</v>
       </c>
       <c r="P19" s="4"/>
@@ -2993,7 +2998,7 @@
       <c r="A20" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="8">
         <v>43555</v>
       </c>
       <c r="C20" s="3"/>
@@ -3027,10 +3032,10 @@
       <c r="M20" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="5">
         <v>92379576</v>
       </c>
-      <c r="O20" t="s" s="5">
+      <c r="O20" t="s" s="6">
         <v>198</v>
       </c>
       <c r="P20" s="4"/>
@@ -3039,7 +3044,7 @@
       <c r="A21" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="8">
         <v>43238</v>
       </c>
       <c r="C21" t="s" s="2">
@@ -3075,13 +3080,13 @@
       <c r="M21" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="N21" s="8">
+      <c r="N21" s="5">
         <v>764686814</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="P21" t="s" s="5">
+      <c r="P21" t="s" s="6">
         <v>209</v>
       </c>
     </row>
@@ -3089,7 +3094,7 @@
       <c r="A22" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="8">
         <v>43018</v>
       </c>
       <c r="C22" t="s" s="2">
@@ -3125,7 +3130,7 @@
       <c r="M22" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N22" s="5">
         <v>2544508314</v>
       </c>
       <c r="O22" s="4"/>
@@ -3135,7 +3140,7 @@
       <c r="A23" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="8">
         <v>39401</v>
       </c>
       <c r="C23" s="4"/>
@@ -3171,7 +3176,7 @@
       <c r="A24" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="8">
         <v>39195</v>
       </c>
       <c r="C24" s="4"/>
@@ -3207,7 +3212,7 @@
       <c r="A25" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="8">
         <v>38860</v>
       </c>
       <c r="C25" s="4"/>
@@ -3243,7 +3248,7 @@
       <c r="A26" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="8">
         <v>39665</v>
       </c>
       <c r="C26" s="4"/>
@@ -3279,7 +3284,7 @@
       <c r="A27" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="8">
         <v>39567</v>
       </c>
       <c r="C27" s="4"/>
@@ -3313,7 +3318,7 @@
       <c r="A28" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="8">
         <v>44919</v>
       </c>
       <c r="C28" s="4"/>
@@ -3349,7 +3354,7 @@
       <c r="A29" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="8">
         <v>44857</v>
       </c>
       <c r="C29" s="3"/>
@@ -3382,14 +3387,14 @@
       <c r="P29" s="4"/>
     </row>
     <row r="30" ht="17" customHeight="1">
-      <c r="A30" s="8">
+      <c r="A30" s="5">
         <v>20211023</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="8">
         <v>44492</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="8">
+      <c r="D30" s="5">
         <v>20211023</v>
       </c>
       <c r="E30" t="s" s="2">
@@ -3421,7 +3426,7 @@
       <c r="A31" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="8">
         <v>44196</v>
       </c>
       <c r="C31" s="3"/>
@@ -3457,7 +3462,7 @@
       <c r="A32" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="8">
         <v>44146</v>
       </c>
       <c r="C32" s="3"/>
@@ -3493,7 +3498,7 @@
       <c r="A33" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="8">
         <v>45153</v>
       </c>
       <c r="C33" t="s" s="2">
@@ -3529,7 +3534,7 @@
       <c r="A34" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="8">
         <v>45281</v>
       </c>
       <c r="C34" s="4"/>

</xml_diff>